<commit_message>
Feat: Test Data 추가 및 소스 개선
+ Test Data 추가 (resources/data/post.json)
+ Entity 내 primitive -> Wrapper 변경
+ Api Separate.

+ Api Docs 및 Sample Data 추가
*참고 site: https://api.stackexchange.com/docs
</commit_message>
<xml_diff>
--- a/src/main/resources/static/References.xlsx
+++ b/src/main/resources/static/References.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sb2ch\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sb2ch\Desktop\backend-ramioverflow\src\main\resources\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F474A2F-B1A8-4DF6-B910-2B784E57659F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD60B3FF-2949-4EEA-B291-B07855392253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B3835AF3-14C7-424F-9038-B7C73F267E5A}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B3835AF3-14C7-424F-9038-B7C73F267E5A}"/>
   </bookViews>
   <sheets>
     <sheet name="api docs" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="175">
   <si>
     <t>/questions</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -144,98 +144,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>PK</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>질문타입
- 1 - 질문
- 2 - 답변</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>채택답변 ID
- - Type이 1일때만</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>부모 ID
- -Type이 2일때만</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>점수</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>조회 수</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>내용</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>최초 생성 일시</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>작성자 ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>작성자 이름</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>최종 수정자 ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>최종 수정자 이름</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>최종 수정 일시</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>제목</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>태그들</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>답변 수</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>좋아요 수</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>댓글 수</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>close 일시</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>close 여부</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>사용 여부</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>삭제 여부</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -407,6 +315,324 @@
   </si>
   <si>
     <t>점수 up 취소</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Question body1 body1 body1 body1 body1 body1 body1 body1 body1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question body2 body2 body2 body2 body2 body2 body2 body2 body2  </t>
+  </si>
+  <si>
+    <t>Question body3 body3 body3 body3 body3 body3 body3 body3 body3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Answer body4 body4 body4 body4 body4 body4 body4 body4 body4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Answer body5 body5 body5 body5 body5 body5 body5 body5 body5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question body6 body6 body6 body6 body6 body6 body6 body6 body6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question body7 body7 body7 body7 body7 body7 body7 body7 body7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Answer body8 body8 body8 body8 body8 body8 body8 body8 body8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question body9 body9 body9 body9 body9 body9 body9 body9 body9 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question body10 body10 body10 body10 body10 body10 body10 body10 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question body11 body11 body11 body11 body11 body11 body11 body11 </t>
+  </si>
+  <si>
+    <t>Answer body12 body12 body12 body12 body12 body12 body12 body12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question body13 body13 body13 body13 body13 body13 body13 body13 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question body14 body14 body14 body14 body14 body14 body14 body14 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Answer body15 body15 body15 body15 body15 body15 body15 body15 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Answer body16 body16 body16 body16 body16 body16 body16 body16 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Answer body17 body17 body17 body17 body17 body17 body17 body17 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Answer body18 body18 body18 body18 body18 body18 body18 body18 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Answer body19 body19 body19 body19 body19 body19 body19 body19 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Answer body20 body20 body20 body20 body20 body20 body20 body20 </t>
+  </si>
+  <si>
+    <t>2022-03-01T11:42:42</t>
+  </si>
+  <si>
+    <t>2022-03-02T07:23:14</t>
+  </si>
+  <si>
+    <t>2022-03-01T20:20:41</t>
+  </si>
+  <si>
+    <t>2022-03-01T18:10:52</t>
+  </si>
+  <si>
+    <t>2022-03-01T19:13:05</t>
+  </si>
+  <si>
+    <t>2022-03-03T11:42:44</t>
+  </si>
+  <si>
+    <t>2022-03-03T13:17:02</t>
+  </si>
+  <si>
+    <t>2022-03-03T16:18:31</t>
+  </si>
+  <si>
+    <t>2022-03-03T22:31:44</t>
+  </si>
+  <si>
+    <t>2022-03-04T07:34:42</t>
+  </si>
+  <si>
+    <t>2022-03-04T08:34:32</t>
+  </si>
+  <si>
+    <t>2022-03-04T09:52:23</t>
+  </si>
+  <si>
+    <t>2022-03-05T10:19:27</t>
+  </si>
+  <si>
+    <t>2022-03-05T19:17:29</t>
+  </si>
+  <si>
+    <t>2022-03-05T22:07:00</t>
+  </si>
+  <si>
+    <t>2022-03-05T23:08:13</t>
+  </si>
+  <si>
+    <t>2022-03-06T02:10:17</t>
+  </si>
+  <si>
+    <t>2022-03-06T07:13:27</t>
+  </si>
+  <si>
+    <t>2022-03-06T09:17:51</t>
+  </si>
+  <si>
+    <t>2022-03-07T00:19:52</t>
+  </si>
+  <si>
+    <t>userId1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>userId2</t>
+  </si>
+  <si>
+    <t>userId3</t>
+  </si>
+  <si>
+    <t>userId4</t>
+  </si>
+  <si>
+    <t>userId5</t>
+  </si>
+  <si>
+    <t>userId6</t>
+  </si>
+  <si>
+    <t>userId7</t>
+  </si>
+  <si>
+    <t>userId8</t>
+  </si>
+  <si>
+    <t>userId9</t>
+  </si>
+  <si>
+    <t>userId10</t>
+  </si>
+  <si>
+    <t>userId11</t>
+  </si>
+  <si>
+    <t>userId12</t>
+  </si>
+  <si>
+    <t>userId13</t>
+  </si>
+  <si>
+    <t>userId14</t>
+  </si>
+  <si>
+    <t>userId15</t>
+  </si>
+  <si>
+    <t>userId16</t>
+  </si>
+  <si>
+    <t>userId17</t>
+  </si>
+  <si>
+    <t>userId18</t>
+  </si>
+  <si>
+    <t>userId19</t>
+  </si>
+  <si>
+    <t>userId20</t>
+  </si>
+  <si>
+    <t>userName1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>userName2</t>
+  </si>
+  <si>
+    <t>userName3</t>
+  </si>
+  <si>
+    <t>userName4</t>
+  </si>
+  <si>
+    <t>userName5</t>
+  </si>
+  <si>
+    <t>userName6</t>
+  </si>
+  <si>
+    <t>userName7</t>
+  </si>
+  <si>
+    <t>userName8</t>
+  </si>
+  <si>
+    <t>userName9</t>
+  </si>
+  <si>
+    <t>userName10</t>
+  </si>
+  <si>
+    <t>userName11</t>
+  </si>
+  <si>
+    <t>userName12</t>
+  </si>
+  <si>
+    <t>userName13</t>
+  </si>
+  <si>
+    <t>userName14</t>
+  </si>
+  <si>
+    <t>userName15</t>
+  </si>
+  <si>
+    <t>userName16</t>
+  </si>
+  <si>
+    <t>userName17</t>
+  </si>
+  <si>
+    <t>userName18</t>
+  </si>
+  <si>
+    <t>userName19</t>
+  </si>
+  <si>
+    <t>userName20</t>
+  </si>
+  <si>
+    <t>what's the betetr between java and c#?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>how can I use jpa in springboot?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>which one is the best in spa lang?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>What is diff in SOAP and REST?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MSA is always better than Monlithic?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>what version of the springboot is nice?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>whichi is more popular language?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Faker is real faker?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Who make the JAVA?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>recommend nice tool for git</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>java;C#</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>jpa;spring;springboot</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>spa;vue;react;angular</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>soap;rest</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>msa;monolithic</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>springboot</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>c;c#;java;node;javascript</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>java</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>git;github;sourcetree</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -468,15 +694,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
@@ -797,7 +1020,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4749CE9A-2403-48F9-BCCE-AF8056861F9C}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -809,20 +1032,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>75</v>
+      <c r="A1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -841,7 +1064,7 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -855,7 +1078,7 @@
         <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -869,7 +1092,7 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -883,7 +1106,7 @@
         <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -897,7 +1120,7 @@
         <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -911,7 +1134,7 @@
         <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="E9">
         <v>2</v>
@@ -925,7 +1148,7 @@
         <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="E10">
         <v>2</v>
@@ -939,7 +1162,7 @@
         <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="E11">
         <v>2</v>
@@ -953,7 +1176,7 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -967,7 +1190,7 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -981,7 +1204,7 @@
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -995,7 +1218,7 @@
         <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -1009,7 +1232,7 @@
         <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -1023,7 +1246,7 @@
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -1039,7 +1262,7 @@
         <v>13</v>
       </c>
       <c r="D19" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -1050,7 +1273,7 @@
         <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -1061,7 +1284,7 @@
         <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -1072,7 +1295,7 @@
         <v>14</v>
       </c>
       <c r="D22" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -1084,7 +1307,7 @@
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="E23">
         <v>2</v>
@@ -1096,7 +1319,7 @@
         <v>23</v>
       </c>
       <c r="D24" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="E24">
         <v>2</v>
@@ -1108,7 +1331,7 @@
         <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="E25">
         <v>2</v>
@@ -1120,7 +1343,7 @@
         <v>25</v>
       </c>
       <c r="D26" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="E26">
         <v>2</v>
@@ -1136,10 +1359,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F385175-2C1A-4C60-BF3C-4698839F62EF}">
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:V21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2:V21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17"/>
@@ -1147,6 +1370,7 @@
     <col min="2" max="2" width="12.58203125" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.58203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" customWidth="1"/>
     <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
@@ -1163,144 +1387,994 @@
     <col min="21" max="22" width="9.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="51">
+    <row r="1" spans="1:22">
       <c r="A1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" t="s">
         <v>38</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" t="s">
         <v>39</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" t="s">
         <v>40</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" t="s">
         <v>42</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" t="s">
         <v>43</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" t="s">
         <v>44</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" t="s">
         <v>45</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" t="s">
         <v>46</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" t="s">
         <v>47</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:22">
-      <c r="A2" t="s">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f ca="1">TRUNC(RAND()*10)</f>
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <f ca="1">TRUNC(RAND()*100)</f>
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I2" t="s">
+        <v>116</v>
+      </c>
+      <c r="J2" t="s">
+        <v>136</v>
+      </c>
+      <c r="N2" t="s">
+        <v>156</v>
+      </c>
+      <c r="O2" t="s">
+        <v>166</v>
+      </c>
+      <c r="P2">
+        <v>2</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="T2" t="b">
+        <v>0</v>
+      </c>
+      <c r="U2" t="b">
+        <v>1</v>
+      </c>
+      <c r="V2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E21" ca="1" si="0">TRUNC(RAND()*10)</f>
+        <v>8</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F21" ca="1" si="1">TRUNC(RAND()*100)</f>
+        <v>53</v>
+      </c>
+      <c r="G3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H3" t="s">
+        <v>97</v>
+      </c>
+      <c r="I3" t="s">
+        <v>117</v>
+      </c>
+      <c r="J3" t="s">
+        <v>137</v>
+      </c>
+      <c r="N3" t="s">
+        <v>157</v>
+      </c>
+      <c r="O3" t="s">
+        <v>167</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>4</v>
+      </c>
+      <c r="T3" t="b">
+        <v>0</v>
+      </c>
+      <c r="U3" t="b">
+        <v>1</v>
+      </c>
+      <c r="V3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ca="1" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="G4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I4" t="s">
+        <v>118</v>
+      </c>
+      <c r="J4" t="s">
+        <v>138</v>
+      </c>
+      <c r="N4" t="s">
+        <v>158</v>
+      </c>
+      <c r="O4" t="s">
+        <v>168</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="T4" t="b">
+        <v>0</v>
+      </c>
+      <c r="U4" t="b">
+        <v>1</v>
+      </c>
+      <c r="V4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H5" t="s">
+        <v>99</v>
+      </c>
+      <c r="I5" t="s">
+        <v>119</v>
+      </c>
+      <c r="J5" t="s">
+        <v>139</v>
+      </c>
+      <c r="T5" t="b">
+        <v>0</v>
+      </c>
+      <c r="U5" t="b">
+        <v>1</v>
+      </c>
+      <c r="V5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ca="1" si="1"/>
+        <v>63</v>
+      </c>
+      <c r="G6" t="s">
+        <v>80</v>
+      </c>
+      <c r="H6" t="s">
+        <v>100</v>
+      </c>
+      <c r="I6" t="s">
+        <v>120</v>
+      </c>
+      <c r="J6" t="s">
+        <v>140</v>
+      </c>
+      <c r="T6" t="b">
+        <v>0</v>
+      </c>
+      <c r="U6" t="b">
+        <v>1</v>
+      </c>
+      <c r="V6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <f t="shared" ca="1" si="1"/>
         <v>49</v>
       </c>
-      <c r="B2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I2" t="s">
-        <v>57</v>
-      </c>
-      <c r="J2" t="s">
-        <v>58</v>
-      </c>
-      <c r="K2" t="s">
-        <v>59</v>
-      </c>
-      <c r="L2" t="s">
-        <v>60</v>
-      </c>
-      <c r="M2" t="s">
-        <v>61</v>
-      </c>
-      <c r="N2" t="s">
-        <v>62</v>
-      </c>
-      <c r="O2" t="s">
-        <v>63</v>
-      </c>
-      <c r="P2" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>65</v>
-      </c>
-      <c r="R2" t="s">
-        <v>66</v>
-      </c>
-      <c r="S2" t="s">
-        <v>67</v>
-      </c>
-      <c r="T2" t="s">
-        <v>68</v>
-      </c>
-      <c r="U2" t="s">
-        <v>69</v>
-      </c>
-      <c r="V2" t="s">
-        <v>70</v>
+      <c r="G7" t="s">
+        <v>81</v>
+      </c>
+      <c r="H7" t="s">
+        <v>101</v>
+      </c>
+      <c r="I7" t="s">
+        <v>121</v>
+      </c>
+      <c r="J7" t="s">
+        <v>141</v>
+      </c>
+      <c r="N7" t="s">
+        <v>159</v>
+      </c>
+      <c r="O7" t="s">
+        <v>169</v>
+      </c>
+      <c r="P7">
+        <v>3</v>
+      </c>
+      <c r="Q7">
+        <v>3</v>
+      </c>
+      <c r="T7" t="b">
+        <v>0</v>
+      </c>
+      <c r="U7" t="b">
+        <v>1</v>
+      </c>
+      <c r="V7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <f t="shared" ca="1" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="G8" t="s">
+        <v>82</v>
+      </c>
+      <c r="H8" t="s">
+        <v>102</v>
+      </c>
+      <c r="I8" t="s">
+        <v>122</v>
+      </c>
+      <c r="J8" t="s">
+        <v>142</v>
+      </c>
+      <c r="N8" t="s">
+        <v>160</v>
+      </c>
+      <c r="O8" t="s">
+        <v>170</v>
+      </c>
+      <c r="P8">
+        <v>3</v>
+      </c>
+      <c r="Q8">
+        <v>2</v>
+      </c>
+      <c r="T8" t="b">
+        <v>0</v>
+      </c>
+      <c r="U8" t="b">
+        <v>1</v>
+      </c>
+      <c r="V8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ca="1" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="G9" t="s">
+        <v>83</v>
+      </c>
+      <c r="H9" t="s">
+        <v>103</v>
+      </c>
+      <c r="I9" t="s">
+        <v>123</v>
+      </c>
+      <c r="J9" t="s">
+        <v>143</v>
+      </c>
+      <c r="T9" t="b">
+        <v>0</v>
+      </c>
+      <c r="U9" t="b">
+        <v>1</v>
+      </c>
+      <c r="V9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <f t="shared" ca="1" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="G10" t="s">
+        <v>84</v>
+      </c>
+      <c r="H10" t="s">
+        <v>104</v>
+      </c>
+      <c r="I10" t="s">
+        <v>124</v>
+      </c>
+      <c r="J10" t="s">
+        <v>144</v>
+      </c>
+      <c r="N10" t="s">
+        <v>161</v>
+      </c>
+      <c r="O10" t="s">
+        <v>171</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>3</v>
+      </c>
+      <c r="T10" t="b">
+        <v>0</v>
+      </c>
+      <c r="U10" t="b">
+        <v>1</v>
+      </c>
+      <c r="V10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <f t="shared" ca="1" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="G11" t="s">
+        <v>85</v>
+      </c>
+      <c r="H11" t="s">
+        <v>105</v>
+      </c>
+      <c r="I11" t="s">
+        <v>125</v>
+      </c>
+      <c r="J11" t="s">
+        <v>145</v>
+      </c>
+      <c r="N11" t="s">
+        <v>162</v>
+      </c>
+      <c r="O11" t="s">
+        <v>172</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="T11" t="b">
+        <v>0</v>
+      </c>
+      <c r="U11" t="b">
+        <v>1</v>
+      </c>
+      <c r="V11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ca="1" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="G12" t="s">
+        <v>86</v>
+      </c>
+      <c r="H12" t="s">
+        <v>106</v>
+      </c>
+      <c r="I12" t="s">
+        <v>126</v>
+      </c>
+      <c r="J12" t="s">
+        <v>146</v>
+      </c>
+      <c r="N12" t="s">
+        <v>163</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>4</v>
+      </c>
+      <c r="T12" t="b">
+        <v>0</v>
+      </c>
+      <c r="U12" t="b">
+        <v>1</v>
+      </c>
+      <c r="V12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>6</v>
+      </c>
+      <c r="E13">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F13">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="G13" t="s">
+        <v>87</v>
+      </c>
+      <c r="H13" t="s">
+        <v>107</v>
+      </c>
+      <c r="I13" t="s">
+        <v>127</v>
+      </c>
+      <c r="J13" t="s">
+        <v>147</v>
+      </c>
+      <c r="T13" t="b">
+        <v>0</v>
+      </c>
+      <c r="U13" t="b">
+        <v>1</v>
+      </c>
+      <c r="V13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F14">
+        <f t="shared" ca="1" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="G14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H14" t="s">
+        <v>108</v>
+      </c>
+      <c r="I14" t="s">
+        <v>128</v>
+      </c>
+      <c r="J14" t="s">
+        <v>148</v>
+      </c>
+      <c r="N14" t="s">
+        <v>164</v>
+      </c>
+      <c r="O14" t="s">
+        <v>173</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>1</v>
+      </c>
+      <c r="T14" t="b">
+        <v>0</v>
+      </c>
+      <c r="U14" t="b">
+        <v>1</v>
+      </c>
+      <c r="V14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F15">
+        <f t="shared" ca="1" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="G15" t="s">
+        <v>89</v>
+      </c>
+      <c r="H15" t="s">
+        <v>109</v>
+      </c>
+      <c r="I15" t="s">
+        <v>129</v>
+      </c>
+      <c r="J15" t="s">
+        <v>149</v>
+      </c>
+      <c r="N15" t="s">
+        <v>165</v>
+      </c>
+      <c r="O15" t="s">
+        <v>174</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="T15" t="b">
+        <v>0</v>
+      </c>
+      <c r="U15" t="b">
+        <v>1</v>
+      </c>
+      <c r="V15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>6</v>
+      </c>
+      <c r="E16">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <f t="shared" ca="1" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="G16" t="s">
+        <v>90</v>
+      </c>
+      <c r="H16" t="s">
+        <v>110</v>
+      </c>
+      <c r="I16" t="s">
+        <v>130</v>
+      </c>
+      <c r="J16" t="s">
+        <v>150</v>
+      </c>
+      <c r="T16" t="b">
+        <v>0</v>
+      </c>
+      <c r="U16" t="b">
+        <v>1</v>
+      </c>
+      <c r="V16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>6</v>
+      </c>
+      <c r="E17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <f t="shared" ca="1" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="G17" t="s">
+        <v>91</v>
+      </c>
+      <c r="H17" t="s">
+        <v>111</v>
+      </c>
+      <c r="I17" t="s">
+        <v>131</v>
+      </c>
+      <c r="J17" t="s">
+        <v>151</v>
+      </c>
+      <c r="T17" t="b">
+        <v>0</v>
+      </c>
+      <c r="U17" t="b">
+        <v>1</v>
+      </c>
+      <c r="V17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>7</v>
+      </c>
+      <c r="E18">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F18">
+        <f t="shared" ca="1" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="G18" t="s">
+        <v>92</v>
+      </c>
+      <c r="H18" t="s">
+        <v>112</v>
+      </c>
+      <c r="I18" t="s">
+        <v>132</v>
+      </c>
+      <c r="J18" t="s">
+        <v>152</v>
+      </c>
+      <c r="T18" t="b">
+        <v>0</v>
+      </c>
+      <c r="U18" t="b">
+        <v>1</v>
+      </c>
+      <c r="V18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>7</v>
+      </c>
+      <c r="E19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="G19" t="s">
+        <v>93</v>
+      </c>
+      <c r="H19" t="s">
+        <v>113</v>
+      </c>
+      <c r="I19" t="s">
+        <v>133</v>
+      </c>
+      <c r="J19" t="s">
+        <v>153</v>
+      </c>
+      <c r="T19" t="b">
+        <v>0</v>
+      </c>
+      <c r="U19" t="b">
+        <v>1</v>
+      </c>
+      <c r="V19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>7</v>
+      </c>
+      <c r="E20">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F20">
+        <f t="shared" ca="1" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="G20" t="s">
+        <v>94</v>
+      </c>
+      <c r="H20" t="s">
+        <v>114</v>
+      </c>
+      <c r="I20" t="s">
+        <v>134</v>
+      </c>
+      <c r="J20" t="s">
+        <v>154</v>
+      </c>
+      <c r="T20" t="b">
+        <v>0</v>
+      </c>
+      <c r="U20" t="b">
+        <v>1</v>
+      </c>
+      <c r="V20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>13</v>
+      </c>
+      <c r="E21">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F21">
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G21" t="s">
+        <v>95</v>
+      </c>
+      <c r="H21" t="s">
+        <v>115</v>
+      </c>
+      <c r="I21" t="s">
+        <v>135</v>
+      </c>
+      <c r="J21" t="s">
+        <v>155</v>
+      </c>
+      <c r="T21" t="b">
+        <v>0</v>
+      </c>
+      <c r="U21" t="b">
+        <v>1</v>
+      </c>
+      <c r="V21" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>